<commit_message>
[example.xlsx] update IosSafariTest data
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Example/example.xlsx
+++ b/src/test/resources/excelData/Example/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\New\SeleniumFramework\src\test\resources\excelData\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C267B38D-5265-4A2B-AA28-BA61ECD8EA90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8920E7A9-56E6-4280-9A5E-5E4BD4B11713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>com.apple.preferences</t>
   </si>
   <si>
-    <t>11.*</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Ahold</t>
+  </si>
+  <si>
+    <t>12.0.*</t>
   </si>
 </sst>
 </file>
@@ -686,10 +686,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -819,7 +821,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>14</v>
@@ -919,13 +921,13 @@
         <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>32</v>
@@ -944,10 +946,10 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -958,13 +960,13 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>33</v>
@@ -993,7 +995,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1028,13 +1030,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
@@ -1066,7 +1068,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1092,11 +1094,11 @@
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>36</v>
@@ -1125,11 +1127,11 @@
         <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>37</v>
@@ -1139,10 +1141,10 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="4"/>
@@ -1162,7 +1164,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1170,7 +1172,7 @@
         <v>38</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1195,7 +1197,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1203,7 +1205,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>

</xml_diff>

<commit_message>
update iOS plaftformVersion for perfecto-gridtype tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Example/example.xlsx
+++ b/src/test/resources/excelData/Example/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\New\SeleniumFramework\src\test\resources\excelData\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8920E7A9-56E6-4280-9A5E-5E4BD4B11713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5E1C3F-5D31-427B-81D4-E24CA88831D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>com.apple.preferences</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>android</t>
-  </si>
-  <si>
     <t>iOS</t>
   </si>
   <si>
@@ -212,6 +206,12 @@
   </si>
   <si>
     <t>12.0.*</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>11.*</t>
   </si>
 </sst>
 </file>
@@ -686,10 +686,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -790,9 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -821,7 +819,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>14</v>
@@ -921,13 +919,13 @@
         <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>32</v>
@@ -946,10 +944,10 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -960,13 +958,13 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>33</v>
@@ -995,7 +993,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1030,13 +1028,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
@@ -1068,7 +1066,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1094,11 +1092,11 @@
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>36</v>
@@ -1127,11 +1125,11 @@
         <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>37</v>
@@ -1141,10 +1139,10 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="4"/>
@@ -1164,16 +1162,16 @@
         <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1197,16 +1195,16 @@
         <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1231,8 +1229,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="G11" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>